<commit_message>
Finished expense class and db operations
</commit_message>
<xml_diff>
--- a/deliverables/ganttChartAvocadoBudget_V4.xlsx
+++ b/deliverables/ganttChartAvocadoBudget_V4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielcronauer/Desktop/ceg4110-group-project-avocadobudget/deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6045765E-0AE4-6C49-8913-9C8540D4C236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91FC449-7951-E746-93E3-05A00C0C32FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-4400" windowWidth="25960" windowHeight="18580" activeTab="4" xr2:uid="{AB48C4DA-0DA3-C24A-B5FB-8C34E6C351BB}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="44">
   <si>
     <t>Team Composition Form</t>
   </si>
@@ -163,9 +163,6 @@
     <t>Expected Start Date</t>
   </si>
   <si>
-    <t>Estimated Date to Complete</t>
-  </si>
-  <si>
     <t>Expected End Date</t>
   </si>
   <si>
@@ -173,6 +170,12 @@
   </si>
   <si>
     <t>Crud Operations</t>
+  </si>
+  <si>
+    <t>Testing / Optional Feature Adds</t>
+  </si>
+  <si>
+    <t>Estimated days to complete task</t>
   </si>
 </sst>
 </file>
@@ -2045,7 +2048,7 @@
                   <c:v>Additional Features as time allows</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Testing / Finalizing</c:v>
+                  <c:v>Testing / Optional Feature Adds</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2180,7 +2183,7 @@
                   <c:v>Additional Features as time allows</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Testing / Finalizing</c:v>
+                  <c:v>Testing / Optional Feature Adds</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2192,7 +2195,7 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7</c:v>
@@ -2222,16 +2225,16 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>7</c:v>
@@ -2550,7 +2553,7 @@
                   <c:v>Additional Features as time allows</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Testing / Finalizing</c:v>
+                  <c:v>Testing / Optional Feature Adds</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2693,7 +2696,7 @@
                   <c:v>Additional Features as time allows</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>Testing / Finalizing</c:v>
+                  <c:v>Testing / Optional Feature Adds</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2705,7 +2708,7 @@
                 <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>45534</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>45541</c:v>
@@ -2735,16 +2738,16 @@
                   <c:v>45583</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41933</c:v>
+                  <c:v>41940</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45595</c:v>
+                  <c:v>45600</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>45595</c:v>
+                  <c:v>45600</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>45600</c:v>
+                  <c:v>45604</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>45607</c:v>
@@ -7963,7 +7966,7 @@
   <dimension ref="A1:X103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:H17"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7994,11 +7997,9 @@
         <v>38</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="3" t="s">
         <v>39</v>
       </c>
+      <c r="H1" s="3"/>
       <c r="I1" s="5">
         <v>1</v>
       </c>
@@ -8045,13 +8046,12 @@
         <f>VLOOKUP(B2,$I:$K,3,FALSE)</f>
         <v>45531</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="8" t="e">
         <f>F2+H2</f>
-        <v>45534</v>
-      </c>
-      <c r="H2" s="9">
-        <f>C2</f>
-        <v>3</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="I2" s="5">
         <v>2</v>
@@ -8367,7 +8367,7 @@
         <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9" s="8">
         <v>45562</v>
@@ -8512,10 +8512,10 @@
       </c>
       <c r="G12" s="8">
         <f t="shared" si="2"/>
-        <v>41933</v>
+        <v>41940</v>
       </c>
       <c r="H12" s="9">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="I12" s="5">
         <v>12</v>
@@ -8553,10 +8553,10 @@
       </c>
       <c r="G13" s="8">
         <f t="shared" si="2"/>
-        <v>45595</v>
+        <v>45600</v>
       </c>
       <c r="H13" s="9">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I13" s="5">
         <v>13</v>
@@ -8583,7 +8583,7 @@
         <v>63</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F14" s="8">
         <f t="shared" si="1"/>
@@ -8591,10 +8591,10 @@
       </c>
       <c r="G14" s="8">
         <f t="shared" si="2"/>
-        <v>45595</v>
+        <v>45600</v>
       </c>
       <c r="H14" s="9">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I14" s="5">
         <v>14</v>
@@ -8628,10 +8628,10 @@
       </c>
       <c r="G15" s="8">
         <f t="shared" si="2"/>
-        <v>45600</v>
+        <v>45604</v>
       </c>
       <c r="H15" s="9">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I15" s="5">
         <v>15</v>
@@ -8697,7 +8697,7 @@
         <v>91</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="F17" s="8">
         <f t="shared" si="1"/>

</xml_diff>